<commit_message>
Worked on the effects doc. + Cleaned the Guardian skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>Additional Info</t>
   </si>
@@ -53,18 +53,9 @@
     <t>[[Modifiable range: No ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 1 ]]</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 3 ]]</t>
   </si>
   <si>
-    <t>[[Boost resistance by 25%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Armor''.</t>
-  </si>
-  <si>
     <t>Omniscient Shield</t>
   </si>
   <si>
@@ -74,30 +65,12 @@
     <t>[[Area of effect: - Every entity]]</t>
   </si>
   <si>
-    <t>Effect name: ''Invulnerable''.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: 6  ]]</t>
-  </si>
-  <si>
-    <t>[[Invulnerable]] (1 turn)</t>
-  </si>
-  <si>
     <t>Backfire</t>
   </si>
   <si>
     <t>[[AP: 5 ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Backfire''.</t>
-  </si>
-  <si>
-    <t>[[Return 20% damage taken]] (1 turns)</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: 3  ]]</t>
-  </si>
-  <si>
     <t>Barricade</t>
   </si>
   <si>
@@ -122,24 +95,12 @@
     <t>[[Area of effect: - 3 cells in horizontal line]]</t>
   </si>
   <si>
-    <t>Summon 3 ''Barricade'' [[15% of guardian max HP, 0 AP, 0 MP, 60% earth resistence, 0% fire resistence, 30% water resistence, 60% air resistence, 100% light resistence, -50% dark resistence]]</t>
-  </si>
-  <si>
     <t>Binding</t>
   </si>
   <si>
     <t>[[MP: 1 ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Binding''.</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Target and adjacent cells]]</t>
-  </si>
-  <si>
-    <t>[[Binding]] (1 turn)</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 4 ]]</t>
   </si>
   <si>
@@ -167,30 +128,12 @@
     <t>Spirit Shield</t>
   </si>
   <si>
-    <t>Summon a ''Gardna'' [[1 HP, 3 AP, 1 MP, 1000% earth resistence, -1000% fire resistence, 1000% water resistence, 1000% air resistence, 1000% light resistence, 1000% dark resistence]]</t>
-  </si>
-  <si>
     <t>[[Number of casts per turn: 1 ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Spirit Shield''.</t>
-  </si>
-  <si>
-    <t>[[Boost  resistance by 15%]] (1 turn)</t>
-  </si>
-  <si>
     <t>Will Of Destruction</t>
   </si>
   <si>
-    <t>Effect name: ''Will Of Destruction''.</t>
-  </si>
-  <si>
-    <t>[[Boost damage by 25%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>[[Reduct resistance by 25%]] (2 turns)</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 8 ]]</t>
   </si>
   <si>
@@ -215,21 +158,6 @@
     <t>[[Range: 1 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  [50 light + 50 earth] + [25 light * MP consumed] ]]</t>
-  </si>
-  <si>
-    <t>[[Boost HP by 20% of max HP of the affected target]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Spirit Fusion''.</t>
-  </si>
-  <si>
-    <t>if not under ''Will Of Destruction'' effect, Self: [[Boost resistance by 15%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>if not under ''Will Of Destruction'' effect, Self: [[Boost HP by 20% of the guardian]] (2 turns)</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Square area around himself]]</t>
   </si>
   <si>
@@ -242,12 +170,6 @@
     <t>[[Number of cast per turn per target: 1 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  25-35 earth ]]</t>
-  </si>
-  <si>
-    <t>If is an enemy, [[Damage:  35-45 earth ]]</t>
-  </si>
-  <si>
     <t>Makes all targets present in the fight invulnerable.                       Can't be used if the caster is under the Will Of Destruction effect.</t>
   </si>
   <si>
@@ -260,47 +182,321 @@
     <t xml:space="preserve"> Summons Barricade on the empty cells in the area of effect.       Can't be used if the caster is under the Will Of Destruction effect.</t>
   </si>
   <si>
-    <t>[[Reduct MP by 100]] (1 turn)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove all the MP of the caster and the target and prevent them to be moved. </t>
-  </si>
-  <si>
     <t>Summons Gardna on the empty cell. The caster can only have one Gardna on the field.                                                                        Can't be used if the caster is under the Will Of Destruction effect.</t>
   </si>
   <si>
-    <t>Increases the resistances and the HP of the caster and his allies in the area of effect.                                                                                     Can't be used if the summoner is under the Will Of Destruction effect.</t>
-  </si>
-  <si>
-    <t>Remove all the protection effect on the caster and his allies. Temporarily transform this skill into the Sword Of Destruction skill. Prevents the usage of the caster protection skills.                         The offensive skill of the caster are changed to Light-type damage. Increases the damage but reduces the resistances.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflicts Light-type and Earth-type damage.                    Consume the remaning MP and for each MP consumed, increase the Light-type damage.                                            This skill is only available when the caster is under the Will Of Destruction effect. </t>
-  </si>
-  <si>
-    <t>Teleport the guardian to the targeted cell.</t>
-  </si>
-  <si>
-    <t>Teleports onto the targeted cell.                                                          If not under the Will Of Destruction effect, increases the resistances and the HP of the caster.                                                                  Can only be used when targeting the caster Gardna.          Unsummon the Gardna.</t>
-  </si>
-  <si>
-    <t>If not under the Will Of Destruction effect, inflicts Earth-type damage, otherwise inflicts Light-type damage in the area of effect.</t>
-  </si>
-  <si>
-    <t>If not under the Will Of Destruction effect, inflicts Earth-type damage to enemies, otherwise inflicts Light-type damage to enemies.                                                                                          Move the caster in front of the target and push it.                           Can only target an entity.</t>
-  </si>
-  <si>
     <t>Push the target by 3 cells.</t>
   </si>
   <si>
-    <t>[[Will Of Destruction]] (2 turns)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Armor]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Invulnerable]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 6 ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Backfire]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 leves (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Summon 3 ''Barricade'' [[15% of caster max HP, 0 AP, 0 MP, 60% ground resistence, 0% fire resistence, 30% water resistence, 60% wind resistence, 100% light resistence, -50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Target and adjacent cells ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Binding]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Slowness]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+10 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove the MP of the caster and the target and prevent them to be moved. </t>
+  </si>
+  <si>
+    <t>Summon a ''Gardna'' [[1 HP, 3 AP, 1 MP, 1000% ground resistence, 1000% fire resistence, 1000% water resistence, 1000% wind resistence, 1000% light resistence, 1000% dark resistence]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Protection Layer]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +1 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vitality]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflicts Light-type and Ground-type damage.                    Consume the remaning MP and for each MP consumed, increase the Light-type damage.                                            This skill is only available when the caster is under the Will Of Destruction effect. </t>
+  </si>
+  <si>
+    <t>[[Damage:  [50 light + 50 ground] + [25 light * MP consumed] ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage to enemies.                                             Move the caster in front of the target and push it.                           Can only target an entity.</t>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage to enemies.</t>
+  </si>
+  <si>
+    <t>[[Damage:  25-35 ground ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Over Power]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vulnerable]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +50 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Will Of Destruction]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove all ''defensive effects''.</t>
+  </si>
+  <si>
+    <t>Remove all the protection effect on the caster.                                Unsummon the Gardna.                                                             Temporarily transform this skill into the Sword Of Destruction skill. Prevents the usage of the caster protection skills.                          Increases the damage but reduces the resistances.</t>
+  </si>
+  <si>
+    <t>Reduces to 0 the damage taken from distance for one hit and increase the HP.</t>
+  </si>
+  <si>
+    <t>Unsummon the Gardna.                                                                    Teleports onto the targeted cell.                                                          Reduces to 0 the damage taken from distance for one hit and increase the HP.                                                                                        Can only be used when targeting the caster Gardna.</t>
+  </si>
+  <si>
+    <t>Teleport to the targeted cell.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Protection Layer]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+1 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vitality]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>On enemy: [[Damage: 35-45 ground ]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +532,24 @@
       <b/>
       <sz val="24"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -429,7 +643,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -471,6 +684,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +1028,7 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1"/>
@@ -819,8 +1040,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>72</v>
+      <c r="C5" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -863,75 +1084,66 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -943,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,8 +1175,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>54</v>
+      <c r="C3" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -973,10 +1185,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>84</v>
+      <c r="C5" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -995,14 +1207,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1014,21 +1226,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1040,14 +1252,14 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1059,26 +1271,26 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>70</v>
+      <c r="C20" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>85</v>
+      <c r="C21" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1107,13 +1319,13 @@
     </row>
     <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1123,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,8 +1357,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1157,8 +1369,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>71</v>
+      <c r="C5" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1170,7 +1382,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1201,75 +1413,66 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1279,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,8 +1504,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>16</v>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1313,8 +1516,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>73</v>
+      <c r="C5" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1326,7 +1529,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1357,75 +1560,66 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1438,7 +1632,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,8 +1653,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>21</v>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1471,8 +1665,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>74</v>
+      <c r="C5" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1484,14 +1678,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1503,21 +1697,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1529,7 +1723,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1541,7 +1735,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1550,10 +1744,10 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
-        <v>29</v>
+      <c r="C18" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1582,7 +1776,7 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1620,8 +1814,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>30</v>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1632,8 +1826,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>76</v>
+      <c r="C5" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1652,7 +1846,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1683,7 +1877,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1695,26 +1889,26 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>34</v>
+      <c r="C17" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>75</v>
+      <c r="C18" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1743,9 +1937,7 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1763,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,8 +1972,8 @@
   <sheetData>
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
-      <c r="G1" s="10" t="s">
-        <v>42</v>
+      <c r="G1" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -1795,13 +1987,13 @@
     </row>
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>36</v>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="7" t="s">
-        <v>43</v>
+      <c r="G3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1813,15 +2005,15 @@
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="20" t="s">
-        <v>77</v>
+      <c r="C5" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="20" t="s">
-        <v>78</v>
+      <c r="G5" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1848,7 +2040,7 @@
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -1868,7 +2060,7 @@
     <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
@@ -1878,7 +2070,7 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -1890,7 +2082,7 @@
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -1903,14 +2095,14 @@
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
@@ -1928,7 +2120,7 @@
     <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
@@ -1945,25 +2137,25 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="78" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
-        <v>44</v>
+      <c r="C18" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="12" t="s">
-        <v>47</v>
+      <c r="G18" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="2:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="9"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="12" t="s">
-        <v>61</v>
+      <c r="G19" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2006,12 +2198,10 @@
     </row>
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="G25" s="7"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -2020,7 +2210,7 @@
       <c r="D26" s="5"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="11"/>
+      <c r="H26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2032,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2231,7 @@
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="2.85546875" customWidth="1"/>
     <col min="7" max="7" width="78.5703125" customWidth="1"/>
     <col min="8" max="8" width="2.85546875" customWidth="1"/>
@@ -2049,8 +2239,8 @@
   <sheetData>
     <row r="1" spans="2:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
-      <c r="G1" s="10" t="s">
-        <v>56</v>
+      <c r="G1" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2064,13 +2254,13 @@
     </row>
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>48</v>
+      <c r="C3" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="7" t="s">
-        <v>57</v>
+      <c r="G3" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2084,13 +2274,13 @@
     </row>
     <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="20" t="s">
-        <v>79</v>
+      <c r="C5" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="19" t="s">
-        <v>80</v>
+      <c r="G5" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2105,12 +2295,12 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -2120,7 +2310,7 @@
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2132,7 +2322,7 @@
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2167,7 +2357,7 @@
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
@@ -2176,68 +2366,68 @@
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>50</v>
+      <c r="C18" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
+      <c r="C19" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>86</v>
+      <c r="C20" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
@@ -2283,12 +2473,10 @@
     </row>
     <row r="26" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="16" t="s">
-        <v>49</v>
-      </c>
+      <c r="C26" s="15"/>
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -2307,10 +2495,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,8 +2517,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="15" t="s">
-        <v>55</v>
+      <c r="C3" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2341,8 +2529,8 @@
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="18" t="s">
-        <v>82</v>
+      <c r="C5" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2361,7 +2549,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2373,21 +2561,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2398,8 +2586,8 @@
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2411,82 +2599,70 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
+      <c r="C18" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="17" t="s">
-        <v>81</v>
+      <c r="C20" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1"/>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="24"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C26" s="12"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="1"/>
-      <c r="C28" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2499,7 +2675,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,8 +2694,8 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
-        <v>53</v>
+      <c r="C3" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2528,10 +2704,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="20" t="s">
-        <v>83</v>
+      <c r="C5" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2543,7 +2719,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2574,7 +2750,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2586,7 +2762,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2598,7 +2774,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2627,13 +2803,13 @@
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="8"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Updated the skills of the Guardian.
- Next task will be to update the Elementalist skills. The core mechanic will be changed.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\_Done\4_Guardian\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sébastien Godbout\Desktop\_MyDev\BattleForVoxturia\GameDesign\Class\_Done\4_Guardian\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="4-Barricade" sheetId="4" r:id="rId4"/>
     <sheet name="5-Binding" sheetId="5" r:id="rId5"/>
     <sheet name="6-Gardna" sheetId="6" r:id="rId6"/>
-    <sheet name="7-WillOfDestruction" sheetId="7" r:id="rId7"/>
+    <sheet name="7-DestructionSword" sheetId="7" r:id="rId7"/>
     <sheet name="8-SpiritFusion" sheetId="8" r:id="rId8"/>
     <sheet name="9-MetallicTornado" sheetId="9" r:id="rId9"/>
     <sheet name="10-DefensiveCharge" sheetId="10" r:id="rId10"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>Additional Info</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Omniscient Shield</t>
   </si>
   <si>
-    <t>[[AP: 6 ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Every entity]]</t>
   </si>
   <si>
@@ -131,12 +128,6 @@
     <t>[[Number of casts per turn: 1 ]]</t>
   </si>
   <si>
-    <t>Will Of Destruction</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: 8 ]]</t>
-  </si>
-  <si>
     <t>Metallic Tornado</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>2nd form skill</t>
   </si>
   <si>
-    <t>Sword Of Destruction</t>
-  </si>
-  <si>
     <t>[[MP: Remaning ]]</t>
   </si>
   <si>
@@ -164,25 +152,7 @@
     <t>[[Number of casts per turn: 2 ]]</t>
   </si>
   <si>
-    <t>[[Range: 2-3 ]]</t>
-  </si>
-  <si>
     <t>[[Number of cast per turn per target: 1 ]]</t>
-  </si>
-  <si>
-    <t>Makes all targets present in the fight invulnerable.                       Can't be used if the caster is under the Will Of Destruction effect.</t>
-  </si>
-  <si>
-    <t>Increases the resistances of the caster and his allies in the area of effect.                                                                                              Can't be used if the caster is under the Will Of Destruction effect.</t>
-  </si>
-  <si>
-    <t>Return a pourcentage of the damage taken of the caster and his allies in the area of effect for the current turn.                                       Can't be used if the caster is under the Will Of Destruction effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Summons Barricade on the empty cells in the area of effect.       Can't be used if the caster is under the Will Of Destruction effect.</t>
-  </si>
-  <si>
-    <t>Summons Gardna on the empty cell. The caster can only have one Gardna on the field.                                                                        Can't be used if the caster is under the Will Of Destruction effect.</t>
   </si>
   <si>
     <t>Push the target by 3 cells.</t>
@@ -290,26 +260,6 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Protection Layer]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +1 level (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
       <t>[[Vitality]]</t>
     </r>
     <r>
@@ -323,9 +273,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Inflicts Light-type and Ground-type damage.                    Consume the remaning MP and for each MP consumed, increase the Light-type damage.                                            This skill is only available when the caster is under the Will Of Destruction effect. </t>
-  </si>
-  <si>
     <t>[[Damage:  [50 light + 50 ground] + [25 light * MP consumed] ]]</t>
   </si>
   <si>
@@ -338,95 +285,10 @@
     <t>[[Damage:  25-35 ground ]]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Will Of Destruction]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>Remove all ''defensive effects''.</t>
-  </si>
-  <si>
-    <t>Remove all the protection effect on the caster.                                Unsummon the Gardna.                                                             Temporarily transform this skill into the Sword Of Destruction skill. Prevents the usage of the caster protection skills.                          Increases the damage but reduces the resistances.</t>
-  </si>
-  <si>
     <t>Reduces to 0 the damage taken from distance for one hit and increase the HP.</t>
   </si>
   <si>
-    <t>Unsummon the Gardna.                                                                    Teleports onto the targeted cell.                                                          Reduces to 0 the damage taken from distance for one hit and increase the HP.                                                                                        Can only be used when targeting the caster Gardna.</t>
-  </si>
-  <si>
     <t>Teleport to the targeted cell.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[[Protection Layer]] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>+1 level (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Vitality]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +20 levels (2 turns)</t>
-    </r>
   </si>
   <si>
     <t>On enemy: [[Damage: 35-45 ground ]]</t>
@@ -452,6 +314,27 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Increases the resistances of the caster and his allies in the area of effect.                                                                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makes all targets present in the fight invulnerable.                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return a pourcentage of the damage taken of the caster and his allies in the area of effect for the current turn.                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Summons Barricade on the empty cells in the area of effect.       </t>
+  </si>
+  <si>
+    <t>[[MP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summons Gardna on the empty cell. The caster can only have one Gardna on the field.                                                                        </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -459,7 +342,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Over-Power]]</t>
+      <t>[[Protection Layer]]</t>
     </r>
     <r>
       <rPr>
@@ -468,10 +351,19 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +25 levels (2 turns)</t>
+      <t xml:space="preserve"> +1 level (1 turn)</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Inflicts Light-type and Ground-type damage.                    Consume the remaning MP and for each MP consumed, increase the Light-type damage.                                            </t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 2 ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Self: </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -479,7 +371,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Vulnerability]]</t>
+      <t>[[Void]]</t>
     </r>
     <r>
       <rPr>
@@ -488,14 +380,35 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +50 levels (2 turns)</t>
+      <t xml:space="preserve"> +25 levels</t>
     </r>
+  </si>
+  <si>
+    <t>Self: End turn.</t>
+  </si>
+  <si>
+    <t>Destructive Sword</t>
+  </si>
+  <si>
+    <t>Unsummon the Gardna.</t>
+  </si>
+  <si>
+    <t>Self: [[Heal: 20% of Max HP ]]</t>
+  </si>
+  <si>
+    <t>Unsummon the Gardna.                                                                    Teleports onto the targeted cell.                                                          Heal the caster.                                                                                      Can only be used when targeting the caster Gardna.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell (The Gardna cell)]]</t>
+  </si>
+  <si>
+    <t>[[Range: 2 ]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -669,9 +582,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -688,10 +598,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,14 +915,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1038,10 +948,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>46</v>
+      <c r="C5" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1084,7 +994,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1108,7 +1018,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1152,14 +1062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1176,7 +1086,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1187,8 +1097,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>64</v>
+      <c r="C5" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1207,14 +1117,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1226,21 +1136,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1252,14 +1162,14 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1271,7 +1181,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1282,15 +1192,15 @@
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="22" t="s">
-        <v>50</v>
+      <c r="C20" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="22" t="s">
-        <v>75</v>
+      <c r="C21" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1325,7 +1235,7 @@
     <row r="28" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1334,14 +1244,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1367,10 +1277,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>45</v>
+      <c r="C5" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1382,7 +1292,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1413,7 +1323,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1425,7 +1335,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1437,7 +1347,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1481,14 +1391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1505,7 +1415,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1514,10 +1424,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>47</v>
+      <c r="C5" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1529,7 +1439,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1584,7 +1494,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1628,14 +1538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1654,7 +1564,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1663,10 +1573,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>48</v>
+      <c r="C5" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1678,14 +1588,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1697,21 +1607,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1723,7 +1633,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1735,7 +1645,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1746,8 +1656,8 @@
     </row>
     <row r="18" spans="2:4" ht="78" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="21" t="s">
-        <v>55</v>
+      <c r="C18" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1791,14 +1701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1815,7 +1725,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1826,8 +1736,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>58</v>
+      <c r="C5" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1839,14 +1749,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1877,7 +1787,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1889,7 +1799,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1900,15 +1810,15 @@
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="22" t="s">
-        <v>76</v>
+      <c r="C17" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="22" t="s">
-        <v>57</v>
+      <c r="C18" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1952,14 +1862,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1973,7 +1883,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -1988,12 +1898,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2005,15 +1915,15 @@
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="19" t="s">
-        <v>49</v>
+      <c r="C5" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="19" t="s">
-        <v>70</v>
+      <c r="G5" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2040,7 +1950,7 @@
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2060,7 +1970,7 @@
     <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
@@ -2070,7 +1980,7 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -2082,7 +1992,7 @@
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -2095,14 +2005,14 @@
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
@@ -2120,7 +2030,7 @@
     <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
@@ -2140,12 +2050,12 @@
     <row r="18" spans="2:8" ht="78" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2155,7 +2065,7 @@
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="11" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2219,273 +2129,171 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="3" max="3" width="78.5703125" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="1"/>
-      <c r="G1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="19" t="s">
-        <v>69</v>
+      <c r="C5" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="22" t="s">
-        <v>68</v>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="22" t="s">
-        <v>67</v>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="22" t="s">
-        <v>77</v>
+      <c r="C19" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="22" t="s">
-        <v>78</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="5"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2494,14 +2302,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2518,7 +2326,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2527,10 +2335,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="17" t="s">
-        <v>71</v>
+      <c r="C5" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2542,14 +2350,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2561,21 +2369,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2587,82 +2395,70 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
+      <c r="C16" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="16" t="s">
-        <v>72</v>
+      <c r="C18" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="1"/>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="22"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="24"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C24" s="12"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="1"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2671,14 +2467,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2695,7 +2491,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2706,8 +2502,8 @@
     </row>
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="19" t="s">
-        <v>65</v>
+      <c r="C5" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2719,7 +2515,7 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2750,7 +2546,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2762,7 +2558,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2774,7 +2570,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2809,7 +2605,7 @@
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Simplified the Elementalist and GrimReaper skills.
- Next class skills to simplify is the Druid.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
+++ b/GameDesign/Class/_Done/4_Guardian/Documentation/GuardianSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-ArmorStrengthening" sheetId="1" r:id="rId1"/>
@@ -1065,7 +1065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1394,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1704,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>